<commit_message>
issue fixed for all the xss
issue fixed for all the xss
</commit_message>
<xml_diff>
--- a/un-admin-server/src/main/resources/static/signature_sheet.xlsx
+++ b/un-admin-server/src/main/resources/static/signature_sheet.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24701"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23FE670D-8A43-4C9F-9A9F-EC164C036781}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD00E289-9BD2-4708-8567-D8FE045EFFFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -74,7 +74,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">+3 ARTS / COMMERCE 2ND YEAR </t>
+      <t>.............................................</t>
     </r>
     <r>
       <rPr>
@@ -155,7 +155,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>2ND (1.00 - 4.00 PM)</t>
+      <t>...................</t>
     </r>
     <r>
       <rPr>
@@ -705,7 +705,7 @@
   <dimension ref="A1:E36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>